<commit_message>
plotting performance across time
</commit_message>
<xml_diff>
--- a/juan/coop_seek_and_find_v2_updated.xlsx
+++ b/juan/coop_seek_and_find_v2_updated.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2106" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2303" uniqueCount="283">
   <si>
     <t>Trainer</t>
   </si>
@@ -694,15 +694,33 @@
     <t>3 drops</t>
   </si>
   <si>
-    <t>b</t>
+    <t>perforated_10_mm/10 pokes</t>
+  </si>
+  <si>
+    <t>solid/ 10 pokes</t>
   </si>
   <si>
     <t>Mistake: I used cooperation lights</t>
   </si>
   <si>
+    <t>perforated_10_mm/ 5 pokes</t>
+  </si>
+  <si>
     <t>pokesPerMouse=5</t>
   </si>
   <si>
+    <t>solid/ 5 pokes</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>perforated_10_mm / dark</t>
+  </si>
+  <si>
+    <t>transparent_no_holes / dark</t>
+  </si>
+  <si>
     <t>Rewarded trials coop024</t>
   </si>
   <si>
@@ -751,10 +769,19 @@
     <t>drops=2</t>
   </si>
   <si>
-    <t>transparent_no_holes / dark</t>
-  </si>
-  <si>
-    <t>perforated_10_mm / dark</t>
+    <t>transparent_no_holes / light</t>
+  </si>
+  <si>
+    <t>Resolution: 960x720</t>
+  </si>
+  <si>
+    <t>Video size: 7.5 GB</t>
+  </si>
+  <si>
+    <t>level 3 of light (max)</t>
+  </si>
+  <si>
+    <t>Resolution: 800x448</t>
   </si>
   <si>
     <t>Rewarded trials coop026</t>
@@ -790,10 +817,58 @@
     <t>Poke = 10.drops=3</t>
   </si>
   <si>
+    <t>first 10 min autolights</t>
+  </si>
+  <si>
+    <t>resolution: 800x448</t>
+  </si>
+  <si>
+    <t>Video size: 2.1 GB</t>
+  </si>
+  <si>
+    <t>start comparison</t>
+  </si>
+  <si>
+    <t>resolution: 1024x576</t>
+  </si>
+  <si>
+    <t>mistake: it should have been dark</t>
+  </si>
+  <si>
+    <t>comparison in light to make recordings</t>
+  </si>
+  <si>
     <t>Rewarded trials coop028</t>
   </si>
   <si>
     <t>Rewarded trials coop029</t>
+  </si>
+  <si>
+    <t>pokePerMouse=5</t>
+  </si>
+  <si>
+    <t>drops =2</t>
+  </si>
+  <si>
+    <t>Resolution: 640x360</t>
+  </si>
+  <si>
+    <t>Video size: 955.8 MB</t>
+  </si>
+  <si>
+    <t>Resolution: 800x600</t>
+  </si>
+  <si>
+    <t>resolution: 1920x1080</t>
+  </si>
+  <si>
+    <t>10 -19 fps/s</t>
+  </si>
+  <si>
+    <t>resolution: 1280x720</t>
+  </si>
+  <si>
+    <t>mistake: run extra 30 min</t>
   </si>
 </sst>
 </file>
@@ -982,7 +1057,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border/>
     <border>
       <left style="thin">
@@ -998,11 +1073,27 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="103">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1288,6 +1379,24 @@
     <xf borderId="1" fillId="12" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1308,7 +1417,7 @@
     <xdr:ext cx="4333875" cy="3257550"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1386,7 +1495,7 @@
     <xdr:ext cx="3781425" cy="3048000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1416,14 +1525,14 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3810000" cy="3000375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1448,19 +1557,47 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3781425" cy="3095625"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4676775" cy="3476625"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image7.png" title="Imagen"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1481,19 +1618,47 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3781425" cy="2962275"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4829175" cy="3600450"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image5.png" title="Imagen"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3005,7 +3170,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="5" max="5" width="15.13"/>
-    <col customWidth="1" min="10" max="10" width="14.13"/>
+    <col customWidth="1" min="10" max="10" width="16.88"/>
     <col customWidth="1" min="12" max="12" width="20.5"/>
   </cols>
   <sheetData>
@@ -3029,10 +3194,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="73" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="H1" s="73" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
       <c r="I1" s="87" t="s">
         <v>7</v>
@@ -3063,7 +3228,7 @@
       <c r="C2" s="5">
         <v>1.0</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="100">
         <v>1.0</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -3079,23 +3244,23 @@
         <v>52.0</v>
       </c>
       <c r="I2" s="8">
-        <f t="shared" ref="I2:I8" si="1">(AVERAGE(G2:H2)/F2)</f>
+        <f t="shared" ref="I2:I30" si="1">(AVERAGE(G2:H2)/F2)</f>
         <v>0.5914634146</v>
       </c>
       <c r="L2" s="16" t="s">
         <v>11</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3">
@@ -3106,10 +3271,10 @@
         <v>45174.0</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" ref="C3:C13" si="2">C2+1</f>
+        <f t="shared" ref="C3:C34" si="2">C2+1</f>
         <v>2</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="100">
         <v>1.0</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -3155,7 +3320,7 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="100">
         <v>1.0</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -3217,6 +3382,9 @@
         <f t="shared" si="1"/>
         <v>0.06546854942</v>
       </c>
+      <c r="J5" s="7" t="s">
+        <v>180</v>
+      </c>
       <c r="L5" s="18" t="s">
         <v>16</v>
       </c>
@@ -3313,13 +3481,13 @@
         <v>23</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>84</v>
+        <v>153</v>
       </c>
       <c r="O7" s="17">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
       <c r="P7" s="17">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="8">
@@ -3356,13 +3524,13 @@
         <v>23</v>
       </c>
       <c r="N8" s="17">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
       <c r="O8" s="17">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
       <c r="P8" s="17">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="9">
@@ -3382,6 +3550,19 @@
       <c r="E9" s="7" t="s">
         <v>146</v>
       </c>
+      <c r="F9" s="7">
+        <v>1009.0</v>
+      </c>
+      <c r="G9" s="7">
+        <v>31.0</v>
+      </c>
+      <c r="I9" s="8">
+        <f t="shared" si="1"/>
+        <v>0.0307234886</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>185</v>
+      </c>
       <c r="L9" s="18" t="s">
         <v>28</v>
       </c>
@@ -3409,6 +3590,25 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
+      <c r="D10" s="90">
+        <v>3.0</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F10" s="7">
+        <v>1114.0</v>
+      </c>
+      <c r="G10" s="7">
+        <v>49.0</v>
+      </c>
+      <c r="I10" s="8">
+        <f t="shared" si="1"/>
+        <v>0.04398563734</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>274</v>
+      </c>
       <c r="L10" s="25" t="s">
         <v>188</v>
       </c>
@@ -3436,6 +3636,22 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
+      <c r="D11" s="90">
+        <v>3.0</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1128.0</v>
+      </c>
+      <c r="G11" s="7">
+        <v>54.0</v>
+      </c>
+      <c r="I11" s="8">
+        <f t="shared" si="1"/>
+        <v>0.04787234043</v>
+      </c>
       <c r="L11" s="25" t="s">
         <v>35</v>
       </c>
@@ -3463,6 +3679,22 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
+      <c r="D12" s="90">
+        <v>3.0</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F12" s="7">
+        <v>997.0</v>
+      </c>
+      <c r="G12" s="7">
+        <v>55.0</v>
+      </c>
+      <c r="I12" s="8">
+        <f t="shared" si="1"/>
+        <v>0.05516549649</v>
+      </c>
       <c r="L12" s="18" t="s">
         <v>37</v>
       </c>
@@ -3490,6 +3722,22 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
+      <c r="D13" s="90">
+        <v>3.0</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" s="7">
+        <v>707.0</v>
+      </c>
+      <c r="G13" s="7">
+        <v>63.0</v>
+      </c>
+      <c r="I13" s="8">
+        <f t="shared" si="1"/>
+        <v>0.08910891089</v>
+      </c>
       <c r="L13" s="29" t="s">
         <v>40</v>
       </c>
@@ -3507,6 +3755,35 @@
       </c>
     </row>
     <row r="14">
+      <c r="A14" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B14" s="4">
+        <v>45185.0</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="D14" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" s="7">
+        <v>693.0</v>
+      </c>
+      <c r="G14" s="7">
+        <v>43.0</v>
+      </c>
+      <c r="I14" s="8">
+        <f t="shared" si="1"/>
+        <v>0.06204906205</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>274</v>
+      </c>
       <c r="L14" s="30" t="s">
         <v>43</v>
       </c>
@@ -3524,6 +3801,32 @@
       </c>
     </row>
     <row r="15">
+      <c r="A15" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B15" s="4">
+        <v>45186.0</v>
+      </c>
+      <c r="C15" s="5">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="D15" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F15" s="7">
+        <v>659.0</v>
+      </c>
+      <c r="G15" s="7">
+        <v>55.0</v>
+      </c>
+      <c r="I15" s="8">
+        <f t="shared" si="1"/>
+        <v>0.08345978756</v>
+      </c>
       <c r="L15" s="33" t="s">
         <v>44</v>
       </c>
@@ -3541,6 +3844,32 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="4">
+        <v>45187.0</v>
+      </c>
+      <c r="C16" s="5">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="D16" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" s="7">
+        <v>685.0</v>
+      </c>
+      <c r="G16" s="7">
+        <v>63.0</v>
+      </c>
+      <c r="I16" s="8">
+        <f t="shared" si="1"/>
+        <v>0.09197080292</v>
+      </c>
       <c r="L16" s="33" t="s">
         <v>46</v>
       </c>
@@ -3548,12 +3877,485 @@
         <v>45069.0</v>
       </c>
       <c r="N16" s="37" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="O16" s="37"/>
     </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="4">
+        <v>45188.0</v>
+      </c>
+      <c r="C17" s="5">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="D17" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" s="7">
+        <v>649.0</v>
+      </c>
+      <c r="G17" s="7">
+        <v>69.0</v>
+      </c>
+      <c r="I17" s="8">
+        <f t="shared" si="1"/>
+        <v>0.1063174114</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="76" t="s">
+        <v>230</v>
+      </c>
+      <c r="B18" s="4">
+        <v>45189.0</v>
+      </c>
+      <c r="C18" s="5">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="D18" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F18" s="7">
+        <v>427.0</v>
+      </c>
+      <c r="G18" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="I18" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="4">
+        <v>45190.0</v>
+      </c>
+      <c r="C19" s="5">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="D19" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F19" s="7">
+        <v>467.0</v>
+      </c>
+      <c r="G19" s="7">
+        <v>55.0</v>
+      </c>
+      <c r="I19" s="8">
+        <f t="shared" si="1"/>
+        <v>0.1177730193</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="4">
+        <v>45191.0</v>
+      </c>
+      <c r="C20" s="5">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="D20" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F20" s="7">
+        <v>859.0</v>
+      </c>
+      <c r="G20" s="7">
+        <v>66.0</v>
+      </c>
+      <c r="I20" s="8">
+        <f t="shared" si="1"/>
+        <v>0.07683352736</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="76" t="s">
+        <v>230</v>
+      </c>
+      <c r="B21" s="4">
+        <v>45192.0</v>
+      </c>
+      <c r="C21" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="D21" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F21" s="7">
+        <v>674.0</v>
+      </c>
+      <c r="G21" s="7">
+        <v>72.0</v>
+      </c>
+      <c r="I21" s="8">
+        <f t="shared" si="1"/>
+        <v>0.1068249258</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B22" s="4">
+        <v>45193.0</v>
+      </c>
+      <c r="C22" s="5">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="D22" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F22" s="7">
+        <v>1132.0</v>
+      </c>
+      <c r="G22" s="7">
+        <v>54.0</v>
+      </c>
+      <c r="I22" s="8">
+        <f t="shared" si="1"/>
+        <v>0.04770318021</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="4">
+        <v>45194.0</v>
+      </c>
+      <c r="C23" s="5">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="D23" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F23" s="7">
+        <v>749.0</v>
+      </c>
+      <c r="G23" s="7">
+        <v>66.0</v>
+      </c>
+      <c r="I23" s="8">
+        <f t="shared" si="1"/>
+        <v>0.08811748999</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="4">
+        <v>45195.0</v>
+      </c>
+      <c r="C24" s="5">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="D24" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F24" s="7">
+        <v>1362.0</v>
+      </c>
+      <c r="G24" s="7">
+        <v>79.0</v>
+      </c>
+      <c r="I24" s="8">
+        <f t="shared" si="1"/>
+        <v>0.05800293686</v>
+      </c>
+      <c r="J24" s="101" t="s">
+        <v>279</v>
+      </c>
+      <c r="L24" s="101" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="4">
+        <v>45196.0</v>
+      </c>
+      <c r="C25" s="5">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="D25" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F25" s="7">
+        <v>925.0</v>
+      </c>
+      <c r="G25" s="7">
+        <v>75.0</v>
+      </c>
+      <c r="I25" s="8">
+        <f t="shared" si="1"/>
+        <v>0.08108108108</v>
+      </c>
+      <c r="J25" s="101" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="4">
+        <v>45197.0</v>
+      </c>
+      <c r="C26" s="5">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="D26" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E26" s="102" t="s">
+        <v>148</v>
+      </c>
+      <c r="F26" s="7">
+        <v>1304.0</v>
+      </c>
+      <c r="G26" s="7">
+        <v>75.0</v>
+      </c>
+      <c r="I26" s="8">
+        <f t="shared" si="1"/>
+        <v>0.05751533742</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="4">
+        <v>45198.0</v>
+      </c>
+      <c r="C27" s="5">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="D27" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="7">
+        <v>805.0</v>
+      </c>
+      <c r="G27" s="7">
+        <v>71.0</v>
+      </c>
+      <c r="I27" s="8">
+        <f t="shared" si="1"/>
+        <v>0.08819875776</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B28" s="4">
+        <v>45199.0</v>
+      </c>
+      <c r="C28" s="5">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="D28" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E28" s="102" t="s">
+        <v>148</v>
+      </c>
+      <c r="F28" s="7">
+        <v>1141.0</v>
+      </c>
+      <c r="G28" s="7">
+        <v>63.0</v>
+      </c>
+      <c r="I28" s="8">
+        <f t="shared" si="1"/>
+        <v>0.05521472393</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="4">
+        <v>45200.0</v>
+      </c>
+      <c r="C29" s="5">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="D29" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F29" s="7">
+        <v>598.0</v>
+      </c>
+      <c r="G29" s="7">
+        <v>75.0</v>
+      </c>
+      <c r="I29" s="8">
+        <f t="shared" si="1"/>
+        <v>0.1254180602</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="4">
+        <v>45201.0</v>
+      </c>
+      <c r="C30" s="5">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="D30" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E30" s="102" t="s">
+        <v>148</v>
+      </c>
+      <c r="F30" s="7">
+        <v>1622.0</v>
+      </c>
+      <c r="G30" s="7">
+        <v>112.0</v>
+      </c>
+      <c r="I30" s="8">
+        <f t="shared" si="1"/>
+        <v>0.06905055487</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="4">
+        <v>45202.0</v>
+      </c>
+      <c r="C31" s="5">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="D31" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" s="4">
+        <v>45203.0</v>
+      </c>
+      <c r="C32" s="5">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="D32" s="95">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" s="4">
+        <v>45204.0</v>
+      </c>
+      <c r="C33" s="5">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="D33" s="95">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" s="4">
+        <v>45205.0</v>
+      </c>
+      <c r="C34" s="5">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="D34" s="95">
+        <v>4.0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="30">
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
@@ -3561,8 +4363,6 @@
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
@@ -3570,6 +4370,22 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -8041,7 +8857,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
+    <tabColor rgb="FFFF0000"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
@@ -12184,6 +13000,7 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
+    <tabColor rgb="FFFF0000"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
@@ -17506,7 +18323,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="5" max="5" width="19.5"/>
+    <col customWidth="1" min="5" max="5" width="21.75"/>
     <col customWidth="1" min="10" max="10" width="15.75"/>
     <col customWidth="1" min="11" max="11" width="13.38"/>
     <col customWidth="1" min="12" max="12" width="20.5"/>
@@ -17610,7 +18427,7 @@
         <v>45099.0</v>
       </c>
       <c r="C3" s="14">
-        <f t="shared" ref="C3:C85" si="2">C2+1</f>
+        <f t="shared" ref="C3:C108" si="2">C2+1</f>
         <v>2</v>
       </c>
       <c r="D3" s="15">
@@ -18331,7 +19148,7 @@
         <v>84.0</v>
       </c>
       <c r="I19" s="8">
-        <f t="shared" ref="I19:I38" si="3">AVERAGE(G19:H19)/F19</f>
+        <f t="shared" ref="I19:I61" si="3">AVERAGE(G19:H19)/F19</f>
         <v>0.121037464</v>
       </c>
     </row>
@@ -18908,8 +19725,9 @@
       <c r="G39" s="89">
         <v>72.0</v>
       </c>
-      <c r="I39" s="48" t="s">
-        <v>224</v>
+      <c r="I39" s="8">
+        <f t="shared" si="3"/>
+        <v>0.1014084507</v>
       </c>
     </row>
     <row r="40">
@@ -18936,7 +19754,7 @@
         <v>77.0</v>
       </c>
       <c r="I40" s="8">
-        <f t="shared" ref="I40:I61" si="4">AVERAGE(G40:H40)/F40</f>
+        <f t="shared" si="3"/>
         <v>0.1230031949</v>
       </c>
     </row>
@@ -18964,7 +19782,7 @@
         <v>57.0</v>
       </c>
       <c r="I41" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.04718543046</v>
       </c>
     </row>
@@ -18992,7 +19810,7 @@
         <v>79.0</v>
       </c>
       <c r="I42" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.09552599758</v>
       </c>
     </row>
@@ -19020,7 +19838,7 @@
         <v>64.0</v>
       </c>
       <c r="I43" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.05609114812</v>
       </c>
     </row>
@@ -19048,7 +19866,7 @@
         <v>85.0</v>
       </c>
       <c r="I44" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.09593679458</v>
       </c>
     </row>
@@ -19076,7 +19894,7 @@
         <v>62.0</v>
       </c>
       <c r="I45" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.05605786618</v>
       </c>
     </row>
@@ -19104,7 +19922,7 @@
         <v>99.0</v>
       </c>
       <c r="I46" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.1287386216</v>
       </c>
       <c r="J46" s="7" t="s">
@@ -19135,7 +19953,7 @@
         <v>57.0</v>
       </c>
       <c r="I47" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.05372290292</v>
       </c>
     </row>
@@ -19163,7 +19981,7 @@
         <v>101.0</v>
       </c>
       <c r="I48" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.150297619</v>
       </c>
     </row>
@@ -19191,7 +20009,7 @@
         <v>59.0</v>
       </c>
       <c r="I49" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.05388127854</v>
       </c>
     </row>
@@ -19210,7 +20028,7 @@
         <v>4.0</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>146</v>
+        <v>224</v>
       </c>
       <c r="F50" s="7">
         <v>740.0</v>
@@ -19219,7 +20037,7 @@
         <v>68.0</v>
       </c>
       <c r="I50" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.09189189189</v>
       </c>
     </row>
@@ -19238,7 +20056,7 @@
         <v>4.0</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="F51" s="7">
         <v>446.0</v>
@@ -19247,7 +20065,7 @@
         <v>5.0</v>
       </c>
       <c r="I51" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.01121076233</v>
       </c>
     </row>
@@ -19266,7 +20084,7 @@
         <v>4.0</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>146</v>
+        <v>224</v>
       </c>
       <c r="F52" s="7">
         <v>432.0</v>
@@ -19275,7 +20093,7 @@
         <v>55.0</v>
       </c>
       <c r="I52" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.1273148148</v>
       </c>
     </row>
@@ -19294,7 +20112,7 @@
         <v>4.0</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="F53" s="7">
         <v>712.0</v>
@@ -19303,7 +20121,7 @@
         <v>7.0</v>
       </c>
       <c r="I53" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.009831460674</v>
       </c>
     </row>
@@ -19322,7 +20140,7 @@
         <v>4.0</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>146</v>
+        <v>224</v>
       </c>
       <c r="F54" s="7">
         <v>689.0</v>
@@ -19331,7 +20149,7 @@
         <v>60.0</v>
       </c>
       <c r="I54" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.08708272859</v>
       </c>
     </row>
@@ -19350,7 +20168,7 @@
         <v>4.0</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="F55" s="7">
         <v>1041.0</v>
@@ -19359,7 +20177,7 @@
         <v>57.0</v>
       </c>
       <c r="I55" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.05475504323</v>
       </c>
     </row>
@@ -19378,7 +20196,7 @@
         <v>4.0</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>146</v>
+        <v>224</v>
       </c>
       <c r="F56" s="7">
         <v>595.0</v>
@@ -19387,7 +20205,7 @@
         <v>58.0</v>
       </c>
       <c r="I56" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.0974789916</v>
       </c>
     </row>
@@ -19406,7 +20224,7 @@
         <v>4.0</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="F57" s="7">
         <v>623.0</v>
@@ -19415,7 +20233,7 @@
         <v>3.0</v>
       </c>
       <c r="I57" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.00481540931</v>
       </c>
     </row>
@@ -19443,11 +20261,11 @@
         <v>130.0</v>
       </c>
       <c r="I58" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.6046511628</v>
       </c>
       <c r="J58" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="59">
@@ -19465,7 +20283,7 @@
         <v>4.0</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>146</v>
+        <v>224</v>
       </c>
       <c r="F59" s="7">
         <v>724.0</v>
@@ -19474,7 +20292,7 @@
         <v>76.0</v>
       </c>
       <c r="I59" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.1049723757</v>
       </c>
     </row>
@@ -19493,7 +20311,7 @@
         <v>4.0</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="F60" s="7">
         <v>949.0</v>
@@ -19502,7 +20320,7 @@
         <v>14.0</v>
       </c>
       <c r="I60" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.01475237092</v>
       </c>
     </row>
@@ -19521,7 +20339,7 @@
         <v>4.0</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>146</v>
+        <v>224</v>
       </c>
       <c r="F61" s="7">
         <v>753.0</v>
@@ -19530,7 +20348,7 @@
         <v>68.0</v>
       </c>
       <c r="I61" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.09030544489</v>
       </c>
     </row>
@@ -19549,7 +20367,7 @@
         <v>4.0</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="G62" s="91"/>
       <c r="I62" s="8"/>
@@ -19569,7 +20387,7 @@
         <v>4.0</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>146</v>
+        <v>224</v>
       </c>
       <c r="F63" s="7">
         <v>651.0</v>
@@ -19578,7 +20396,7 @@
         <v>87.0</v>
       </c>
       <c r="I63" s="8">
-        <f t="shared" ref="I63:I67" si="5">AVERAGE(G63:H63)/F63</f>
+        <f t="shared" ref="I63:I67" si="4">AVERAGE(G63:H63)/F63</f>
         <v>0.133640553</v>
       </c>
     </row>
@@ -19597,7 +20415,7 @@
         <v>4.0</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="F64" s="7">
         <v>1241.0</v>
@@ -19606,7 +20424,7 @@
         <v>58.0</v>
       </c>
       <c r="I64" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.04673650282</v>
       </c>
     </row>
@@ -19625,7 +20443,7 @@
         <v>4.0</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>146</v>
+        <v>227</v>
       </c>
       <c r="F65" s="7">
         <v>725.0</v>
@@ -19634,11 +20452,11 @@
         <v>71.0</v>
       </c>
       <c r="I65" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.09793103448</v>
       </c>
       <c r="J65" s="7" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="66">
@@ -19656,7 +20474,7 @@
         <v>4.0</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="F66" s="7">
         <v>1282.0</v>
@@ -19665,7 +20483,7 @@
         <v>68.0</v>
       </c>
       <c r="I66" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.05304212168</v>
       </c>
     </row>
@@ -19684,7 +20502,7 @@
         <v>4.0</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>146</v>
+        <v>227</v>
       </c>
       <c r="F67" s="7">
         <v>773.0</v>
@@ -19693,7 +20511,7 @@
         <v>79.0</v>
       </c>
       <c r="I67" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.1021992238</v>
       </c>
     </row>
@@ -19752,7 +20570,7 @@
         <v>4.0</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="F70" s="7">
         <v>1398.0</v>
@@ -19761,7 +20579,7 @@
         <v>68.0</v>
       </c>
       <c r="I70" s="8">
-        <f t="shared" ref="I70:I74" si="6">AVERAGE(G70:H70)/F70</f>
+        <f t="shared" ref="I70:I74" si="5">AVERAGE(G70:H70)/F70</f>
         <v>0.04864091559</v>
       </c>
     </row>
@@ -19780,7 +20598,7 @@
         <v>4.0</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>146</v>
+        <v>227</v>
       </c>
       <c r="F71" s="7">
         <v>715.0</v>
@@ -19789,7 +20607,7 @@
         <v>84.0</v>
       </c>
       <c r="I71" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.1174825175</v>
       </c>
     </row>
@@ -19808,7 +20626,7 @@
         <v>4.0</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="F72" s="7">
         <v>964.0</v>
@@ -19817,7 +20635,7 @@
         <v>94.0</v>
       </c>
       <c r="I72" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.09751037344</v>
       </c>
     </row>
@@ -19836,7 +20654,7 @@
         <v>4.0</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>146</v>
+        <v>227</v>
       </c>
       <c r="F73" s="7">
         <v>684.0</v>
@@ -19845,7 +20663,7 @@
         <v>96.0</v>
       </c>
       <c r="I73" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.1403508772</v>
       </c>
     </row>
@@ -19864,7 +20682,7 @@
         <v>4.0</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="F74" s="7">
         <v>972.0</v>
@@ -19873,7 +20691,7 @@
         <v>102.0</v>
       </c>
       <c r="I74" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.1049382716</v>
       </c>
     </row>
@@ -19932,7 +20750,7 @@
         <v>4.0</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>146</v>
+        <v>227</v>
       </c>
       <c r="F77" s="7">
         <v>848.0</v>
@@ -19941,7 +20759,7 @@
         <v>109.0</v>
       </c>
       <c r="I77" s="8">
-        <f t="shared" ref="I77:I81" si="7">AVERAGE(G77:H77)/F77</f>
+        <f t="shared" ref="I77:I81" si="6">AVERAGE(G77:H77)/F77</f>
         <v>0.1285377358</v>
       </c>
     </row>
@@ -19960,7 +20778,7 @@
         <v>4.0</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="F78" s="7">
         <v>1161.0</v>
@@ -19969,7 +20787,7 @@
         <v>100.0</v>
       </c>
       <c r="I78" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.08613264427</v>
       </c>
     </row>
@@ -19988,7 +20806,7 @@
         <v>4.0</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="F79" s="7">
         <v>1159.0</v>
@@ -19997,7 +20815,7 @@
         <v>96.0</v>
       </c>
       <c r="I79" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.08283002588</v>
       </c>
     </row>
@@ -20016,7 +20834,7 @@
         <v>4.0</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>146</v>
+        <v>227</v>
       </c>
       <c r="F80" s="7">
         <v>922.0</v>
@@ -20025,7 +20843,7 @@
         <v>114.0</v>
       </c>
       <c r="I80" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.1236442516</v>
       </c>
     </row>
@@ -20044,7 +20862,7 @@
         <v>4.0</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>146</v>
+        <v>227</v>
       </c>
       <c r="F81" s="7">
         <v>752.0</v>
@@ -20053,7 +20871,7 @@
         <v>116.0</v>
       </c>
       <c r="I81" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.1542553191</v>
       </c>
     </row>
@@ -20075,6 +20893,7 @@
         <v>111</v>
       </c>
       <c r="G82" s="91"/>
+      <c r="I82" s="8"/>
     </row>
     <row r="83">
       <c r="A83" s="7" t="s">
@@ -20094,6 +20913,7 @@
         <v>111</v>
       </c>
       <c r="G83" s="91"/>
+      <c r="I83" s="8"/>
     </row>
     <row r="84">
       <c r="A84" s="7" t="s">
@@ -20110,9 +20930,18 @@
         <v>4.0</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="G84" s="91"/>
+        <v>229</v>
+      </c>
+      <c r="F84" s="7">
+        <v>1063.0</v>
+      </c>
+      <c r="G84" s="89">
+        <v>91.0</v>
+      </c>
+      <c r="I84" s="8">
+        <f t="shared" ref="I84:I88" si="7">AVERAGE(G84:H84)/F84</f>
+        <v>0.08560677328</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="7" t="s">
@@ -20129,53 +20958,596 @@
         <v>4.0</v>
       </c>
       <c r="E85" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F85" s="7">
+        <v>769.0</v>
+      </c>
+      <c r="G85" s="89">
+        <v>111.0</v>
+      </c>
+      <c r="I85" s="8">
+        <f t="shared" si="7"/>
+        <v>0.144343303</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86" s="4">
+        <v>45182.0</v>
+      </c>
+      <c r="C86" s="14">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="D86" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="F86" s="7">
+        <v>930.0</v>
+      </c>
+      <c r="G86" s="89">
+        <v>105.0</v>
+      </c>
+      <c r="I86" s="8">
+        <f t="shared" si="7"/>
+        <v>0.1129032258</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87" s="4">
+        <v>45183.0</v>
+      </c>
+      <c r="C87" s="14">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
+      <c r="D87" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E87" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="G85" s="91"/>
-    </row>
-    <row r="86">
-      <c r="G86" s="91"/>
-    </row>
-    <row r="87">
-      <c r="G87" s="91"/>
+      <c r="F87" s="7">
+        <v>691.0</v>
+      </c>
+      <c r="G87" s="89">
+        <v>99.0</v>
+      </c>
+      <c r="I87" s="8">
+        <f t="shared" si="7"/>
+        <v>0.1432706223</v>
+      </c>
+      <c r="J87" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B88" s="4">
+        <v>45184.0</v>
+      </c>
+      <c r="C88" s="14">
+        <f t="shared" si="2"/>
+        <v>87</v>
+      </c>
+      <c r="D88" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F88" s="7">
+        <v>1227.0</v>
+      </c>
+      <c r="G88" s="89">
+        <v>69.0</v>
+      </c>
+      <c r="I88" s="8">
+        <f t="shared" si="7"/>
+        <v>0.05623471883</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B89" s="4">
+        <v>45185.0</v>
+      </c>
+      <c r="C89" s="14">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+      <c r="D89" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G89" s="91"/>
+      <c r="I89" s="8"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" s="4">
+        <v>45186.0</v>
+      </c>
+      <c r="C90" s="14">
+        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
+      <c r="D90" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G90" s="91"/>
+      <c r="I90" s="8"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91" s="4">
+        <v>45187.0</v>
+      </c>
+      <c r="C91" s="14">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="D91" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F91" s="7">
+        <v>638.0</v>
+      </c>
+      <c r="G91" s="89">
+        <v>108.0</v>
+      </c>
+      <c r="I91" s="8">
+        <f t="shared" ref="I91:I95" si="8">AVERAGE(G91:H91)/F91</f>
+        <v>0.1692789969</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B92" s="4">
+        <v>45188.0</v>
+      </c>
+      <c r="C92" s="14">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
+      <c r="D92" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F92" s="7">
+        <v>1259.0</v>
+      </c>
+      <c r="G92" s="89">
+        <v>74.0</v>
+      </c>
+      <c r="I92" s="8">
+        <f t="shared" si="8"/>
+        <v>0.05877680699</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B93" s="4">
+        <v>45189.0</v>
+      </c>
+      <c r="C93" s="14">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="D93" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F93" s="7">
+        <v>704.0</v>
+      </c>
+      <c r="G93" s="89">
+        <v>95.0</v>
+      </c>
+      <c r="I93" s="8">
+        <f t="shared" si="8"/>
+        <v>0.1349431818</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B94" s="4">
+        <v>45190.0</v>
+      </c>
+      <c r="C94" s="14">
+        <f t="shared" si="2"/>
+        <v>93</v>
+      </c>
+      <c r="D94" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F94" s="7">
+        <v>1122.0</v>
+      </c>
+      <c r="G94" s="89">
+        <v>69.0</v>
+      </c>
+      <c r="I94" s="8">
+        <f t="shared" si="8"/>
+        <v>0.0614973262</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B95" s="4">
+        <v>45191.0</v>
+      </c>
+      <c r="C95" s="14">
+        <f t="shared" si="2"/>
+        <v>94</v>
+      </c>
+      <c r="D95" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F95" s="7">
+        <v>716.0</v>
+      </c>
+      <c r="G95" s="89">
+        <v>90.0</v>
+      </c>
+      <c r="I95" s="8">
+        <f t="shared" si="8"/>
+        <v>0.125698324</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B96" s="4">
+        <v>45192.0</v>
+      </c>
+      <c r="C96" s="14">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+      <c r="D96" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G96" s="91"/>
+      <c r="I96" s="8"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B97" s="4">
+        <v>45193.0</v>
+      </c>
+      <c r="C97" s="14">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+      <c r="D97" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G97" s="91"/>
+      <c r="I97" s="8"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" s="4">
+        <v>45194.0</v>
+      </c>
+      <c r="C98" s="14">
+        <f t="shared" si="2"/>
+        <v>97</v>
+      </c>
+      <c r="D98" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="F98" s="7">
+        <v>880.0</v>
+      </c>
+      <c r="G98" s="89">
+        <v>84.0</v>
+      </c>
+      <c r="I98" s="8">
+        <f t="shared" ref="I98:I102" si="9">AVERAGE(G98:H98)/F98</f>
+        <v>0.09545454545</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" s="4">
+        <v>45195.0</v>
+      </c>
+      <c r="C99" s="14">
+        <f t="shared" si="2"/>
+        <v>98</v>
+      </c>
+      <c r="D99" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F99" s="7">
+        <v>1155.0</v>
+      </c>
+      <c r="G99" s="89">
+        <v>73.0</v>
+      </c>
+      <c r="I99" s="8">
+        <f t="shared" si="9"/>
+        <v>0.0632034632</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B100" s="4">
+        <v>45196.0</v>
+      </c>
+      <c r="C100" s="14">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="D100" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="F100" s="7">
+        <v>740.0</v>
+      </c>
+      <c r="G100" s="89">
+        <v>78.0</v>
+      </c>
+      <c r="I100" s="8">
+        <f t="shared" si="9"/>
+        <v>0.1054054054</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B101" s="4">
+        <v>45197.0</v>
+      </c>
+      <c r="C101" s="14">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="D101" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E101" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F101" s="7">
+        <v>1107.0</v>
+      </c>
+      <c r="G101" s="89">
+        <v>52.0</v>
+      </c>
+      <c r="I101" s="8">
+        <f t="shared" si="9"/>
+        <v>0.04697380307</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B102" s="4">
+        <v>45198.0</v>
+      </c>
+      <c r="C102" s="14">
+        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
+      <c r="D102" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="F102" s="7">
+        <v>794.0</v>
+      </c>
+      <c r="G102" s="89">
+        <v>95.0</v>
+      </c>
+      <c r="I102" s="8">
+        <f t="shared" si="9"/>
+        <v>0.1196473552</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B103" s="4">
+        <v>45199.0</v>
+      </c>
+      <c r="C103" s="14">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+      <c r="D103" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E103" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G103" s="91"/>
+      <c r="I103" s="8"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B104" s="4">
+        <v>45200.0</v>
+      </c>
+      <c r="C104" s="14">
+        <f t="shared" si="2"/>
+        <v>103</v>
+      </c>
+      <c r="D104" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G104" s="91"/>
+      <c r="I104" s="8"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B105" s="4">
+        <v>45201.0</v>
+      </c>
+      <c r="C105" s="14">
+        <f t="shared" si="2"/>
+        <v>104</v>
+      </c>
+      <c r="D105" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F105" s="7">
+        <v>1044.0</v>
+      </c>
+      <c r="G105" s="89">
+        <v>63.0</v>
+      </c>
+      <c r="I105" s="8">
+        <f>AVERAGE(G105:H105)/F105</f>
+        <v>0.06034482759</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B106" s="4">
+        <v>45202.0</v>
+      </c>
+      <c r="C106" s="14">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+      <c r="D106" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="G106" s="91"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B107" s="4">
+        <v>45203.0</v>
+      </c>
+      <c r="C107" s="14">
+        <f t="shared" si="2"/>
+        <v>106</v>
+      </c>
+      <c r="D107" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="G107" s="91"/>
+    </row>
+    <row r="108">
+      <c r="B108" s="4">
+        <v>45204.0</v>
+      </c>
+      <c r="C108" s="14">
+        <f t="shared" si="2"/>
+        <v>107</v>
+      </c>
+      <c r="D108" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="G108" s="91"/>
+    </row>
+    <row r="109">
+      <c r="G109" s="91"/>
+    </row>
+    <row r="110">
+      <c r="G110" s="91"/>
+    </row>
+    <row r="111">
+      <c r="G111" s="91"/>
+    </row>
+    <row r="112">
+      <c r="G112" s="91"/>
     </row>
   </sheetData>
-  <mergeCells count="84">
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="G82:H82"/>
-    <mergeCell ref="G83:H83"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="G87:H87"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="G76:H76"/>
-    <mergeCell ref="G77:H77"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="G79:H79"/>
-    <mergeCell ref="G80:H80"/>
+  <mergeCells count="109">
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
@@ -20225,6 +21597,66 @@
     <mergeCell ref="G50:H50"/>
     <mergeCell ref="G51:H51"/>
     <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G109:H109"/>
+    <mergeCell ref="G110:H110"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="G112:H112"/>
+    <mergeCell ref="G102:H102"/>
+    <mergeCell ref="G103:H103"/>
+    <mergeCell ref="G104:H104"/>
+    <mergeCell ref="G105:H105"/>
+    <mergeCell ref="G106:H106"/>
+    <mergeCell ref="G107:H107"/>
+    <mergeCell ref="G108:H108"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="G82:H82"/>
+    <mergeCell ref="G83:H83"/>
+    <mergeCell ref="G84:H84"/>
+    <mergeCell ref="G85:H85"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="G87:H87"/>
+    <mergeCell ref="G88:H88"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="G90:H90"/>
+    <mergeCell ref="G91:H91"/>
+    <mergeCell ref="G92:H92"/>
+    <mergeCell ref="G93:H93"/>
+    <mergeCell ref="G94:H94"/>
+    <mergeCell ref="G95:H95"/>
+    <mergeCell ref="G96:H96"/>
+    <mergeCell ref="G97:H97"/>
+    <mergeCell ref="G98:H98"/>
+    <mergeCell ref="G99:H99"/>
+    <mergeCell ref="G100:H100"/>
+    <mergeCell ref="G101:H101"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -20241,6 +21673,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="5" max="5" width="21.75"/>
+    <col customWidth="1" min="10" max="10" width="18.25"/>
     <col customWidth="1" min="13" max="13" width="20.5"/>
     <col customWidth="1" min="14" max="17" width="16.5"/>
   </cols>
@@ -20265,10 +21698,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="73" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="H1" s="73" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="I1" s="87" t="s">
         <v>7</v>
@@ -20322,16 +21755,16 @@
         <v>11</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="Q2" s="17" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3">
@@ -20342,7 +21775,7 @@
         <v>45147.0</v>
       </c>
       <c r="C3" s="14">
-        <f t="shared" ref="C3:C36" si="2">C2+1</f>
+        <f t="shared" ref="C3:C59" si="2">C2+1</f>
         <v>2</v>
       </c>
       <c r="D3" s="15">
@@ -20454,7 +21887,7 @@
         <v>0.3134796238</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="M5" s="18" t="s">
         <v>16</v>
@@ -20500,7 +21933,7 @@
         <v>0.08988764045</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="M6" s="25" t="s">
         <v>183</v>
@@ -20546,7 +21979,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="M7" s="25" t="s">
         <v>22</v>
@@ -20592,7 +22025,7 @@
         <v>0.08361204013</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="M8" s="26" t="s">
         <v>26</v>
@@ -20638,7 +22071,7 @@
         <v>0.04933586338</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="M9" s="18" t="s">
         <v>28</v>
@@ -20684,7 +22117,7 @@
         <v>0.04314159292</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="M10" s="25" t="s">
         <v>188</v>
@@ -20730,7 +22163,7 @@
         <v>0.05415499533</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="M11" s="25" t="s">
         <v>35</v>
@@ -20776,7 +22209,7 @@
         <v>0.07079646018</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="M12" s="18" t="s">
         <v>37</v>
@@ -20822,7 +22255,7 @@
         <v>0.04121863799</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="M13" s="29" t="s">
         <v>40</v>
@@ -20868,7 +22301,7 @@
         <v>0.06492248062</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="M14" s="30" t="s">
         <v>43</v>
@@ -20914,7 +22347,7 @@
         <v>0.04931506849</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="M15" s="33" t="s">
         <v>44</v>
@@ -20960,14 +22393,14 @@
         <v>0.07522123894</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="M16" s="33" t="s">
         <v>46</v>
       </c>
       <c r="N16" s="77"/>
       <c r="O16" s="37" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="P16" s="37"/>
     </row>
@@ -20999,7 +22432,7 @@
         <v>0.08945260347</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18">
@@ -21142,7 +22575,7 @@
         <v>0.1304926764</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23">
@@ -21413,7 +22846,7 @@
         <v>48.0</v>
       </c>
       <c r="I32" s="8">
-        <f t="shared" ref="I32:I35" si="3">(AVERAGE(G32:H32)/F32)</f>
+        <f t="shared" ref="I32:I54" si="3">(AVERAGE(G32:H32)/F32)</f>
         <v>0.0359012715</v>
       </c>
     </row>
@@ -21432,7 +22865,7 @@
         <v>4.0</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="F33" s="7">
         <v>1010.0</v>
@@ -21460,7 +22893,7 @@
         <v>4.0</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="F34" s="7">
         <v>797.0</v>
@@ -21488,7 +22921,7 @@
         <v>4.0</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="F35" s="7">
         <v>1044.0</v>
@@ -21516,42 +22949,678 @@
         <v>4.0</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="G36" s="91"/>
+        <v>231</v>
+      </c>
+      <c r="F36" s="7">
+        <v>624.0</v>
+      </c>
+      <c r="G36" s="89">
+        <v>97.0</v>
+      </c>
+      <c r="I36" s="8">
+        <f t="shared" si="3"/>
+        <v>0.1554487179</v>
+      </c>
     </row>
     <row r="37">
-      <c r="G37" s="91"/>
+      <c r="A37" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="4">
+        <v>45181.0</v>
+      </c>
+      <c r="C37" s="14">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="D37" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F37" s="7">
+        <v>784.0</v>
+      </c>
+      <c r="G37" s="89">
+        <v>64.0</v>
+      </c>
+      <c r="I37" s="8">
+        <f t="shared" si="3"/>
+        <v>0.08163265306</v>
+      </c>
     </row>
     <row r="38">
-      <c r="G38" s="91"/>
+      <c r="A38" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="4">
+        <v>45182.0</v>
+      </c>
+      <c r="C38" s="14">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="D38" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="F38" s="7">
+        <v>582.0</v>
+      </c>
+      <c r="G38" s="89">
+        <v>108.0</v>
+      </c>
+      <c r="I38" s="8">
+        <f t="shared" si="3"/>
+        <v>0.1855670103</v>
+      </c>
     </row>
     <row r="39">
-      <c r="G39" s="91"/>
+      <c r="A39" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="4">
+        <v>45183.0</v>
+      </c>
+      <c r="C39" s="14">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="D39" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F39" s="7">
+        <v>1113.0</v>
+      </c>
+      <c r="G39" s="89">
+        <v>97.0</v>
+      </c>
+      <c r="I39" s="8">
+        <f t="shared" si="3"/>
+        <v>0.08715184187</v>
+      </c>
     </row>
     <row r="40">
-      <c r="G40" s="91"/>
+      <c r="A40" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="4">
+        <v>45184.0</v>
+      </c>
+      <c r="C40" s="14">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="D40" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="F40" s="7">
+        <v>640.0</v>
+      </c>
+      <c r="G40" s="89">
+        <v>96.0</v>
+      </c>
+      <c r="I40" s="8">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
+      </c>
     </row>
     <row r="41">
-      <c r="G41" s="91"/>
+      <c r="A41" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B41" s="4">
+        <v>45185.0</v>
+      </c>
+      <c r="C41" s="14">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="D41" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F41" s="7">
+        <v>918.0</v>
+      </c>
+      <c r="G41" s="89">
+        <v>98.0</v>
+      </c>
+      <c r="I41" s="8">
+        <f t="shared" si="3"/>
+        <v>0.1067538126</v>
+      </c>
     </row>
     <row r="42">
-      <c r="G42" s="91"/>
+      <c r="A42" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B42" s="4">
+        <v>45186.0</v>
+      </c>
+      <c r="C42" s="14">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="D42" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="F42" s="7">
+        <v>761.0</v>
+      </c>
+      <c r="G42" s="89">
+        <v>99.0</v>
+      </c>
+      <c r="I42" s="8">
+        <f t="shared" si="3"/>
+        <v>0.1300919842</v>
+      </c>
     </row>
     <row r="43">
-      <c r="G43" s="91"/>
+      <c r="A43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="4">
+        <v>45187.0</v>
+      </c>
+      <c r="C43" s="14">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="D43" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F43" s="7">
+        <v>885.0</v>
+      </c>
+      <c r="G43" s="89">
+        <v>85.0</v>
+      </c>
+      <c r="I43" s="8">
+        <f t="shared" si="3"/>
+        <v>0.09604519774</v>
+      </c>
     </row>
     <row r="44">
-      <c r="G44" s="91"/>
+      <c r="A44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="4">
+        <v>45188.0</v>
+      </c>
+      <c r="C44" s="14">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="D44" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="F44" s="7">
+        <v>703.0</v>
+      </c>
+      <c r="G44" s="89">
+        <v>91.0</v>
+      </c>
+      <c r="I44" s="8">
+        <f t="shared" si="3"/>
+        <v>0.1294452347</v>
+      </c>
     </row>
     <row r="45">
-      <c r="G45" s="91"/>
+      <c r="A45" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B45" s="4">
+        <v>45189.0</v>
+      </c>
+      <c r="C45" s="14">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="D45" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F45" s="7">
+        <v>780.0</v>
+      </c>
+      <c r="G45" s="89">
+        <v>74.0</v>
+      </c>
+      <c r="I45" s="8">
+        <f t="shared" si="3"/>
+        <v>0.09487179487</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="4">
+        <v>45190.0</v>
+      </c>
+      <c r="C46" s="14">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="D46" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F46" s="7">
+        <v>625.0</v>
+      </c>
+      <c r="G46" s="89">
+        <v>51.0</v>
+      </c>
+      <c r="I46" s="8">
+        <f t="shared" si="3"/>
+        <v>0.0816</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" s="4">
+        <v>45191.0</v>
+      </c>
+      <c r="C47" s="14">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="D47" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F47" s="7">
+        <v>884.0</v>
+      </c>
+      <c r="G47" s="89">
+        <v>52.0</v>
+      </c>
+      <c r="I47" s="8">
+        <f t="shared" si="3"/>
+        <v>0.05882352941</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B48" s="4">
+        <v>45192.0</v>
+      </c>
+      <c r="C48" s="14">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="D48" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F48" s="7">
+        <v>747.0</v>
+      </c>
+      <c r="G48" s="89">
+        <v>41.0</v>
+      </c>
+      <c r="I48" s="8">
+        <f t="shared" si="3"/>
+        <v>0.05488621151</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="K48" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B49" s="4">
+        <v>45193.0</v>
+      </c>
+      <c r="C49" s="14">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="D49" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F49" s="7">
+        <v>1015.0</v>
+      </c>
+      <c r="G49" s="89">
+        <v>25.0</v>
+      </c>
+      <c r="I49" s="8">
+        <f t="shared" si="3"/>
+        <v>0.02463054187</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="4">
+        <v>45194.0</v>
+      </c>
+      <c r="C50" s="14">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="D50" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F50" s="7">
+        <v>862.0</v>
+      </c>
+      <c r="G50" s="89">
+        <v>48.0</v>
+      </c>
+      <c r="I50" s="8">
+        <f t="shared" si="3"/>
+        <v>0.05568445476</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="4">
+        <v>45195.0</v>
+      </c>
+      <c r="C51" s="14">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="D51" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F51" s="7">
+        <v>698.0</v>
+      </c>
+      <c r="G51" s="89">
+        <v>45.0</v>
+      </c>
+      <c r="I51" s="8">
+        <f t="shared" si="3"/>
+        <v>0.06446991404</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="K51" s="7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="4">
+        <v>45196.0</v>
+      </c>
+      <c r="C52" s="14">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="D52" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F52" s="7">
+        <v>690.0</v>
+      </c>
+      <c r="G52" s="89">
+        <v>31.0</v>
+      </c>
+      <c r="I52" s="8">
+        <f t="shared" si="3"/>
+        <v>0.04492753623</v>
+      </c>
+      <c r="J52" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" s="4">
+        <v>45197.0</v>
+      </c>
+      <c r="C53" s="14">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="D53" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F53" s="7">
+        <v>599.0</v>
+      </c>
+      <c r="G53" s="89">
+        <v>64.0</v>
+      </c>
+      <c r="I53" s="8">
+        <f t="shared" si="3"/>
+        <v>0.1068447412</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="4">
+        <v>45198.0</v>
+      </c>
+      <c r="C54" s="14">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="D54" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F54" s="7">
+        <v>687.0</v>
+      </c>
+      <c r="G54" s="89">
+        <v>106.0</v>
+      </c>
+      <c r="I54" s="8">
+        <f t="shared" si="3"/>
+        <v>0.154294032</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="4">
+        <v>45199.0</v>
+      </c>
+      <c r="C55" s="14">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="D55" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G55" s="91"/>
+      <c r="I55" s="8"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" s="4">
+        <v>45200.0</v>
+      </c>
+      <c r="C56" s="14">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="D56" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G56" s="91"/>
+      <c r="I56" s="8"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="4">
+        <v>45201.0</v>
+      </c>
+      <c r="C57" s="14">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="D57" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F57" s="7">
+        <v>668.0</v>
+      </c>
+      <c r="G57" s="89">
+        <v>49.0</v>
+      </c>
+      <c r="I57" s="8">
+        <f>(AVERAGE(G57:H57)/F57)</f>
+        <v>0.07335329341</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="4">
+        <v>45202.0</v>
+      </c>
+      <c r="C58" s="14">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="D58" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G58" s="91"/>
+    </row>
+    <row r="59">
+      <c r="B59" s="4">
+        <v>45203.0</v>
+      </c>
+      <c r="C59" s="14">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="D59" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="G59" s="91"/>
+    </row>
+    <row r="60">
+      <c r="G60" s="91"/>
+    </row>
+    <row r="61">
+      <c r="G61" s="91"/>
+    </row>
+    <row r="62">
+      <c r="G62" s="91"/>
+    </row>
+    <row r="63">
+      <c r="G63" s="91"/>
+    </row>
+    <row r="64">
+      <c r="G64" s="91"/>
+    </row>
+    <row r="65">
+      <c r="G65" s="91"/>
+    </row>
+    <row r="66">
+      <c r="G66" s="91"/>
+    </row>
+    <row r="67">
+      <c r="G67" s="91"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="63">
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="G60:H60"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
@@ -21580,12 +23649,6 @@
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G45:H45"/>
     <mergeCell ref="G33:H33"/>
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="G35:H35"/>
@@ -21593,6 +23656,20 @@
     <mergeCell ref="G37:H37"/>
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G53:H53"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -21609,6 +23686,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="5" max="5" width="21.75"/>
+    <col customWidth="1" min="10" max="10" width="15.75"/>
     <col customWidth="1" min="13" max="13" width="20.5"/>
   </cols>
   <sheetData>
@@ -21632,10 +23710,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="73" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="H1" s="73" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="I1" s="87" t="s">
         <v>7</v>
@@ -21689,16 +23767,16 @@
         <v>11</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="Q2" s="17" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3">
@@ -21709,7 +23787,7 @@
         <v>45147.0</v>
       </c>
       <c r="C3" s="14">
-        <f t="shared" ref="C3:C37" si="2">C2+1</f>
+        <f t="shared" ref="C3:C60" si="2">C2+1</f>
         <v>2</v>
       </c>
       <c r="D3" s="15">
@@ -21821,7 +23899,7 @@
         <v>0.09290322581</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="M5" s="18" t="s">
         <v>16</v>
@@ -21867,7 +23945,7 @@
         <v>0.09449760766</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="M6" s="25" t="s">
         <v>183</v>
@@ -21913,7 +23991,7 @@
         <v>0.06090373281</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="M7" s="25" t="s">
         <v>22</v>
@@ -21959,7 +24037,7 @@
         <v>0.0527325024</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="M8" s="26" t="s">
         <v>26</v>
@@ -22005,7 +24083,7 @@
         <v>0.07843137255</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="M9" s="18" t="s">
         <v>28</v>
@@ -22051,7 +24129,7 @@
         <v>0.05448717949</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="M10" s="25" t="s">
         <v>188</v>
@@ -22097,7 +24175,7 @@
         <v>0.0797752809</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="M11" s="25" t="s">
         <v>35</v>
@@ -22143,7 +24221,7 @@
         <v>0.1052631579</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="M12" s="18" t="s">
         <v>37</v>
@@ -22189,7 +24267,7 @@
         <v>0.09417596035</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="M13" s="29" t="s">
         <v>40</v>
@@ -22235,7 +24313,7 @@
         <v>0.1331403763</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="M14" s="30" t="s">
         <v>43</v>
@@ -22330,7 +24408,7 @@
         <v>45041.0</v>
       </c>
       <c r="O16" s="37" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="P16" s="37"/>
     </row>
@@ -22800,7 +24878,7 @@
         <v>4.0</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="F33" s="7">
         <v>338.0</v>
@@ -22812,6 +24890,9 @@
         <f t="shared" si="1"/>
         <v>0.008875739645</v>
       </c>
+      <c r="J33" s="23" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
@@ -22830,6 +24911,7 @@
       <c r="E34" s="7" t="s">
         <v>111</v>
       </c>
+      <c r="I34" s="8"/>
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
@@ -22848,6 +24930,7 @@
       <c r="E35" s="7" t="s">
         <v>111</v>
       </c>
+      <c r="I35" s="8"/>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
@@ -22864,7 +24947,17 @@
         <v>4.0</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>244</v>
+        <v>231</v>
+      </c>
+      <c r="F36" s="7">
+        <v>490.0</v>
+      </c>
+      <c r="G36" s="7">
+        <v>98.0</v>
+      </c>
+      <c r="I36" s="8">
+        <f t="shared" ref="I36:I57" si="3">(AVERAGE(G36:H36)/F36)</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="37">
@@ -22882,11 +24975,668 @@
         <v>4.0</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>243</v>
+        <v>232</v>
+      </c>
+      <c r="F37" s="7">
+        <v>1080.0</v>
+      </c>
+      <c r="G37" s="7">
+        <v>60.0</v>
+      </c>
+      <c r="I37" s="8">
+        <f t="shared" si="3"/>
+        <v>0.05555555556</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="4">
+        <v>45182.0</v>
+      </c>
+      <c r="C38" s="14">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="D38" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="F38" s="7">
+        <v>433.0</v>
+      </c>
+      <c r="G38" s="7">
+        <v>97.0</v>
+      </c>
+      <c r="I38" s="8">
+        <f t="shared" si="3"/>
+        <v>0.2240184758</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="4">
+        <v>45183.0</v>
+      </c>
+      <c r="C39" s="14">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="D39" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F39" s="7">
+        <v>757.0</v>
+      </c>
+      <c r="G39" s="7">
+        <v>59.0</v>
+      </c>
+      <c r="I39" s="8">
+        <f t="shared" si="3"/>
+        <v>0.07793923382</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="4">
+        <v>45184.0</v>
+      </c>
+      <c r="C40" s="14">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="D40" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="F40" s="7">
+        <v>351.0</v>
+      </c>
+      <c r="G40" s="7">
+        <v>82.0</v>
+      </c>
+      <c r="I40" s="8">
+        <f t="shared" si="3"/>
+        <v>0.2336182336</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B41" s="4">
+        <v>45185.0</v>
+      </c>
+      <c r="C41" s="14">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="D41" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F41" s="7">
+        <v>823.0</v>
+      </c>
+      <c r="G41" s="7">
+        <v>65.0</v>
+      </c>
+      <c r="I41" s="8">
+        <f t="shared" si="3"/>
+        <v>0.07897934386</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B42" s="4">
+        <v>45186.0</v>
+      </c>
+      <c r="C42" s="14">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="D42" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="F42" s="7">
+        <v>440.0</v>
+      </c>
+      <c r="G42" s="7">
+        <v>99.0</v>
+      </c>
+      <c r="I42" s="8">
+        <f t="shared" si="3"/>
+        <v>0.225</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="4">
+        <v>45187.0</v>
+      </c>
+      <c r="C43" s="14">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="D43" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F43" s="7">
+        <v>911.0</v>
+      </c>
+      <c r="G43" s="7">
+        <v>82.0</v>
+      </c>
+      <c r="I43" s="8">
+        <f t="shared" si="3"/>
+        <v>0.09001097695</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="4">
+        <v>45188.0</v>
+      </c>
+      <c r="C44" s="14">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="D44" s="97">
+        <v>4.0</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="F44" s="7">
+        <v>569.0</v>
+      </c>
+      <c r="G44" s="7">
+        <v>102.0</v>
+      </c>
+      <c r="I44" s="8">
+        <f t="shared" si="3"/>
+        <v>0.1792618629</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B45" s="4">
+        <v>45189.0</v>
+      </c>
+      <c r="C45" s="14">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="D45" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F45" s="7">
+        <v>897.0</v>
+      </c>
+      <c r="G45" s="7">
+        <v>111.0</v>
+      </c>
+      <c r="I45" s="8">
+        <f t="shared" si="3"/>
+        <v>0.1237458194</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="4">
+        <v>45190.0</v>
+      </c>
+      <c r="C46" s="14">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="D46" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F46" s="7">
+        <v>653.0</v>
+      </c>
+      <c r="G46" s="7">
+        <v>90.0</v>
+      </c>
+      <c r="I46" s="8">
+        <f t="shared" si="3"/>
+        <v>0.1378254211</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" s="4">
+        <v>45191.0</v>
+      </c>
+      <c r="C47" s="14">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="D47" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F47" s="7">
+        <v>711.0</v>
+      </c>
+      <c r="G47" s="7">
+        <v>98.0</v>
+      </c>
+      <c r="I47" s="8">
+        <f t="shared" si="3"/>
+        <v>0.1378340366</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B48" s="4">
+        <v>45192.0</v>
+      </c>
+      <c r="C48" s="14">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="D48" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F48" s="7">
+        <v>600.0</v>
+      </c>
+      <c r="G48" s="7">
+        <v>81.0</v>
+      </c>
+      <c r="I48" s="8">
+        <f t="shared" si="3"/>
+        <v>0.135</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="K48" s="99" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B49" s="4">
+        <v>45193.0</v>
+      </c>
+      <c r="C49" s="14">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="D49" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F49" s="7">
+        <v>709.0</v>
+      </c>
+      <c r="G49" s="7">
+        <v>103.0</v>
+      </c>
+      <c r="I49" s="8">
+        <f t="shared" si="3"/>
+        <v>0.1452750353</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="4">
+        <v>45194.0</v>
+      </c>
+      <c r="C50" s="14">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="D50" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F50" s="7">
+        <v>679.0</v>
+      </c>
+      <c r="G50" s="7">
+        <v>72.0</v>
+      </c>
+      <c r="I50" s="8">
+        <f t="shared" si="3"/>
+        <v>0.1060382916</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="4">
+        <v>45195.0</v>
+      </c>
+      <c r="C51" s="14">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="D51" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F51" s="7">
+        <v>581.0</v>
+      </c>
+      <c r="G51" s="7">
+        <v>93.0</v>
+      </c>
+      <c r="I51" s="8">
+        <f t="shared" si="3"/>
+        <v>0.1600688468</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="K51" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="4">
+        <v>45196.0</v>
+      </c>
+      <c r="C52" s="14">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="D52" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F52" s="7">
+        <v>1046.0</v>
+      </c>
+      <c r="G52" s="7">
+        <v>100.0</v>
+      </c>
+      <c r="I52" s="8">
+        <f t="shared" si="3"/>
+        <v>0.09560229446</v>
+      </c>
+      <c r="K52" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" s="4">
+        <v>45197.0</v>
+      </c>
+      <c r="C53" s="14">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="D53" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F53" s="7">
+        <v>802.0</v>
+      </c>
+      <c r="G53" s="7">
+        <v>99.0</v>
+      </c>
+      <c r="I53" s="8">
+        <f t="shared" si="3"/>
+        <v>0.1234413965</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="4">
+        <v>45198.0</v>
+      </c>
+      <c r="C54" s="14">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="D54" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F54" s="7">
+        <v>502.0</v>
+      </c>
+      <c r="G54" s="7">
+        <v>106.0</v>
+      </c>
+      <c r="I54" s="8">
+        <f t="shared" si="3"/>
+        <v>0.2111553785</v>
+      </c>
+      <c r="J54" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="76" t="s">
+        <v>230</v>
+      </c>
+      <c r="B55" s="4">
+        <v>45199.0</v>
+      </c>
+      <c r="C55" s="14">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="D55" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F55" s="7">
+        <v>772.0</v>
+      </c>
+      <c r="G55" s="7">
+        <v>94.0</v>
+      </c>
+      <c r="I55" s="8">
+        <f t="shared" si="3"/>
+        <v>0.121761658</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="76" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" s="4">
+        <v>45200.0</v>
+      </c>
+      <c r="C56" s="14">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="D56" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F56" s="7">
+        <v>561.0</v>
+      </c>
+      <c r="G56" s="7">
+        <v>86.0</v>
+      </c>
+      <c r="I56" s="8">
+        <f t="shared" si="3"/>
+        <v>0.1532976827</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="4">
+        <v>45201.0</v>
+      </c>
+      <c r="C57" s="14">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="D57" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F57" s="7">
+        <v>423.0</v>
+      </c>
+      <c r="G57" s="7">
+        <v>86.0</v>
+      </c>
+      <c r="I57" s="8">
+        <f t="shared" si="3"/>
+        <v>0.2033096927</v>
+      </c>
+      <c r="J57" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="4">
+        <v>45202.0</v>
+      </c>
+      <c r="C58" s="14">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="D58" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" s="4">
+        <v>45203.0</v>
+      </c>
+      <c r="C59" s="14">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="D59" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J59" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" s="4">
+        <v>45204.0</v>
+      </c>
+      <c r="C60" s="14">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="D60" s="98">
+        <v>4.0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="64">
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="G60:H60"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
@@ -22915,8 +25665,6 @@
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
     <mergeCell ref="G33:H33"/>
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="G35:H35"/>
@@ -22924,6 +25672,20 @@
     <mergeCell ref="G37:H37"/>
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G53:H53"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
adding script for the length of the session in coop project
</commit_message>
<xml_diff>
--- a/juan/coop_seek_and_find_v2_updated.xlsx
+++ b/juan/coop_seek_and_find_v2_updated.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2391" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2445" uniqueCount="294">
   <si>
     <t>Trainer</t>
   </si>
@@ -724,6 +724,9 @@
     <t>transparent_no_holes / light</t>
   </si>
   <si>
+    <t>drop</t>
+  </si>
+  <si>
     <t>Rewarded trials coop024</t>
   </si>
   <si>
@@ -896,6 +899,9 @@
   </si>
   <si>
     <t>diyar</t>
+  </si>
+  <si>
+    <t>extra 10 min</t>
   </si>
 </sst>
 </file>
@@ -1447,7 +1453,7 @@
     <xdr:ext cx="4333875" cy="3257550"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image11.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1480,7 +1486,7 @@
     <xdr:ext cx="4200525" cy="3143250"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image13.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image12.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1521,7 +1527,7 @@
     <xdr:ext cx="3752850" cy="2962275"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1554,7 +1560,7 @@
     <xdr:ext cx="3781425" cy="3048000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1591,7 +1597,7 @@
     <xdr:ext cx="3810000" cy="3000375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1619,7 +1625,7 @@
     <xdr:ext cx="4695825" cy="3000375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image13.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1647,7 +1653,7 @@
     <xdr:ext cx="5829300" cy="3000375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1675,7 +1681,7 @@
     <xdr:ext cx="4448175" cy="3819525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1708,7 +1714,7 @@
     <xdr:ext cx="3781425" cy="3095625"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1736,7 +1742,7 @@
     <xdr:ext cx="4676775" cy="3476625"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1769,7 +1775,7 @@
     <xdr:ext cx="2743200" cy="2152650"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1825,7 +1831,7 @@
     <xdr:ext cx="3829050" cy="2924175"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image10.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3365,10 +3371,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="73" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H1" s="73" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="I1" s="87" t="s">
         <v>7</v>
@@ -3415,23 +3421,23 @@
         <v>52.0</v>
       </c>
       <c r="I2" s="8">
-        <f t="shared" ref="I2:I40" si="1">(AVERAGE(G2:H2)/F2)</f>
+        <f t="shared" ref="I2:I45" si="1">(AVERAGE(G2:H2)/F2)</f>
         <v>0.5914634146</v>
       </c>
       <c r="L2" s="16" t="s">
         <v>11</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3">
@@ -3442,7 +3448,7 @@
         <v>45174.0</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" ref="C3:C41" si="2">C2+1</f>
+        <f t="shared" ref="C3:C47" si="2">C2+1</f>
         <v>2</v>
       </c>
       <c r="D3" s="100">
@@ -3778,7 +3784,7 @@
         <v>0.04398563734</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="L10" s="25" t="s">
         <v>188</v>
@@ -3953,7 +3959,7 @@
         <v>0.06204906205</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="L14" s="30" t="s">
         <v>43</v>
@@ -4048,7 +4054,7 @@
         <v>45069.0</v>
       </c>
       <c r="N16" s="37" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="O16" s="37"/>
     </row>
@@ -4080,7 +4086,7 @@
         <v>0.1063174114</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18">
@@ -4195,10 +4201,10 @@
         <v>0.1068249258</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="22">
@@ -4257,7 +4263,7 @@
         <v>0.08811748999</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="24">
@@ -4288,10 +4294,10 @@
         <v>0.05800293686</v>
       </c>
       <c r="J24" s="101" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L24" s="101" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="25">
@@ -4322,7 +4328,7 @@
         <v>0.08108108108</v>
       </c>
       <c r="J25" s="101" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26">
@@ -4468,7 +4474,7 @@
         <v>0.06905055487</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31">
@@ -4583,10 +4589,10 @@
         <v>0.1105845182</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="35">
@@ -4617,7 +4623,7 @@
         <v>0.1061946903</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="36">
@@ -4648,7 +4654,7 @@
         <v>0.1024691358</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="37">
@@ -4679,7 +4685,7 @@
         <v>0.1077170418</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38">
@@ -4740,7 +4746,7 @@
     </row>
     <row r="40">
       <c r="A40" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B40" s="4">
         <v>45211.0</v>
@@ -4783,29 +4789,181 @@
       <c r="E41" s="7" t="s">
         <v>146</v>
       </c>
+      <c r="F41" s="7">
+        <v>657.0</v>
+      </c>
+      <c r="G41" s="7">
+        <v>59.0</v>
+      </c>
+      <c r="I41" s="8">
+        <f t="shared" si="1"/>
+        <v>0.0898021309</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="42">
+      <c r="A42" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="B42" s="4">
         <v>45213.0</v>
       </c>
+      <c r="C42" s="5">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="D42" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F42" s="7">
+        <v>570.0</v>
+      </c>
+      <c r="G42" s="7">
+        <v>91.0</v>
+      </c>
+      <c r="I42" s="8">
+        <f t="shared" si="1"/>
+        <v>0.1596491228</v>
+      </c>
     </row>
     <row r="43">
+      <c r="A43" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="B43" s="4">
         <v>45214.0</v>
       </c>
+      <c r="C43" s="5">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="D43" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F43" s="7">
+        <v>843.0</v>
+      </c>
+      <c r="G43" s="7">
+        <v>55.0</v>
+      </c>
+      <c r="I43" s="8">
+        <f t="shared" si="1"/>
+        <v>0.06524317912</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="44">
+      <c r="A44" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="B44" s="4">
         <v>45215.0</v>
       </c>
+      <c r="C44" s="5">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="D44" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F44" s="7">
+        <v>1098.0</v>
+      </c>
+      <c r="G44" s="7">
+        <v>13.0</v>
+      </c>
+      <c r="I44" s="8">
+        <f t="shared" si="1"/>
+        <v>0.01183970856</v>
+      </c>
     </row>
     <row r="45">
+      <c r="A45" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="B45" s="4">
         <v>45216.0</v>
       </c>
+      <c r="C45" s="5">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="D45" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F45" s="7">
+        <v>572.0</v>
+      </c>
+      <c r="G45" s="7">
+        <v>43.0</v>
+      </c>
+      <c r="I45" s="8">
+        <f t="shared" si="1"/>
+        <v>0.07517482517</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="4">
+        <v>45217.0</v>
+      </c>
+      <c r="C46" s="5">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="D46" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" s="4">
+        <v>45218.0</v>
+      </c>
+      <c r="C47" s="5">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="D47" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="D48" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="57">
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
@@ -4834,12 +4992,6 @@
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G45:H45"/>
     <mergeCell ref="G33:H33"/>
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="G35:H35"/>
@@ -4847,6 +4999,28 @@
     <mergeCell ref="G37:H37"/>
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G53:H53"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -18888,7 +19062,7 @@
         <v>45099.0</v>
       </c>
       <c r="C3" s="14">
-        <f t="shared" ref="C3:C117" si="2">C2+1</f>
+        <f t="shared" ref="C3:C119" si="2">C2+1</f>
         <v>2</v>
       </c>
       <c r="D3" s="15">
@@ -22123,7 +22297,7 @@
         <v>66.0</v>
       </c>
       <c r="I112" s="8">
-        <f t="shared" ref="I112:I115" si="11">AVERAGE(G112:H112)/F112</f>
+        <f t="shared" ref="I112:I116" si="11">AVERAGE(G112:H112)/F112</f>
         <v>0.06303724928</v>
       </c>
     </row>
@@ -22228,7 +22402,16 @@
       <c r="E116" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="G116" s="91"/>
+      <c r="F116" s="7">
+        <v>1067.0</v>
+      </c>
+      <c r="G116" s="89">
+        <v>47.0</v>
+      </c>
+      <c r="I116" s="8">
+        <f t="shared" si="11"/>
+        <v>0.04404873477</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="7" t="s">
@@ -22245,18 +22428,126 @@
         <v>4.0</v>
       </c>
       <c r="E117" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G117" s="91"/>
+      <c r="I117" s="8"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B118" s="4">
+        <v>45214.0</v>
+      </c>
+      <c r="C118" s="14">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+      <c r="D118" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E118" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G118" s="91"/>
+      <c r="I118" s="8"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B119" s="4">
+        <v>45215.0</v>
+      </c>
+      <c r="C119" s="14">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+      <c r="D119" s="69">
+        <v>4.0</v>
+      </c>
+      <c r="E119" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="G117" s="91"/>
-    </row>
-    <row r="118">
-      <c r="G118" s="91"/>
-    </row>
-    <row r="119">
-      <c r="G119" s="91"/>
+      <c r="F119" s="7">
+        <v>963.0</v>
+      </c>
+      <c r="G119" s="89">
+        <v>72.0</v>
+      </c>
+      <c r="I119" s="8">
+        <f>AVERAGE(G119:H119)/F119</f>
+        <v>0.07476635514</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D120" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="F120" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="G120" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="H120" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="I120" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="J120" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="G121" s="91"/>
+    </row>
+    <row r="122">
+      <c r="G122" s="91"/>
+    </row>
+    <row r="123">
+      <c r="G123" s="91"/>
+    </row>
+    <row r="124">
+      <c r="G124" s="91"/>
+    </row>
+    <row r="125">
+      <c r="G125" s="91"/>
+    </row>
+    <row r="126">
+      <c r="G126" s="91"/>
+    </row>
+    <row r="127">
+      <c r="G127" s="91"/>
+    </row>
+    <row r="128">
+      <c r="G128" s="91"/>
+    </row>
+    <row r="129">
+      <c r="G129" s="91"/>
+    </row>
+    <row r="130">
+      <c r="G130" s="91"/>
+    </row>
+    <row r="131">
+      <c r="G131" s="91"/>
     </row>
   </sheetData>
-  <mergeCells count="116">
+  <mergeCells count="127">
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
@@ -22313,10 +22604,6 @@
     <mergeCell ref="G106:H106"/>
     <mergeCell ref="G107:H107"/>
     <mergeCell ref="G108:H108"/>
-    <mergeCell ref="G116:H116"/>
-    <mergeCell ref="G117:H117"/>
-    <mergeCell ref="G118:H118"/>
-    <mergeCell ref="G119:H119"/>
     <mergeCell ref="G109:H109"/>
     <mergeCell ref="G110:H110"/>
     <mergeCell ref="G111:H111"/>
@@ -22324,6 +22611,21 @@
     <mergeCell ref="G113:H113"/>
     <mergeCell ref="G114:H114"/>
     <mergeCell ref="G115:H115"/>
+    <mergeCell ref="G124:H124"/>
+    <mergeCell ref="G125:H125"/>
+    <mergeCell ref="G126:H126"/>
+    <mergeCell ref="G127:H127"/>
+    <mergeCell ref="G128:H128"/>
+    <mergeCell ref="G129:H129"/>
+    <mergeCell ref="G130:H130"/>
+    <mergeCell ref="G131:H131"/>
+    <mergeCell ref="G116:H116"/>
+    <mergeCell ref="G117:H117"/>
+    <mergeCell ref="G118:H118"/>
+    <mergeCell ref="G119:H119"/>
+    <mergeCell ref="G121:H121"/>
+    <mergeCell ref="G122:H122"/>
+    <mergeCell ref="G123:H123"/>
     <mergeCell ref="G53:H53"/>
     <mergeCell ref="G54:H54"/>
     <mergeCell ref="G55:H55"/>
@@ -22414,10 +22716,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="73" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H1" s="73" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="I1" s="87" t="s">
         <v>7</v>
@@ -22471,16 +22773,16 @@
         <v>11</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="Q2" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3">
@@ -22491,7 +22793,7 @@
         <v>45147.0</v>
       </c>
       <c r="C3" s="14">
-        <f t="shared" ref="C3:C69" si="2">C2+1</f>
+        <f t="shared" ref="C3:C76" si="2">C2+1</f>
         <v>2</v>
       </c>
       <c r="D3" s="15">
@@ -22603,7 +22905,7 @@
         <v>0.3134796238</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="M5" s="18" t="s">
         <v>16</v>
@@ -22649,7 +22951,7 @@
         <v>0.08988764045</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="M6" s="25" t="s">
         <v>183</v>
@@ -22695,7 +22997,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M7" s="25" t="s">
         <v>22</v>
@@ -22741,7 +23043,7 @@
         <v>0.08361204013</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M8" s="26" t="s">
         <v>26</v>
@@ -22787,7 +23089,7 @@
         <v>0.04933586338</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="M9" s="18" t="s">
         <v>28</v>
@@ -22833,7 +23135,7 @@
         <v>0.04314159292</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="M10" s="25" t="s">
         <v>188</v>
@@ -22879,7 +23181,7 @@
         <v>0.05415499533</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="M11" s="25" t="s">
         <v>35</v>
@@ -22925,7 +23227,7 @@
         <v>0.07079646018</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="M12" s="18" t="s">
         <v>37</v>
@@ -22971,7 +23273,7 @@
         <v>0.04121863799</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="M13" s="29" t="s">
         <v>40</v>
@@ -23017,7 +23319,7 @@
         <v>0.06492248062</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M14" s="30" t="s">
         <v>43</v>
@@ -23063,7 +23365,7 @@
         <v>0.04931506849</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="M15" s="33" t="s">
         <v>44</v>
@@ -23109,14 +23411,14 @@
         <v>0.07522123894</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="M16" s="33" t="s">
         <v>46</v>
       </c>
       <c r="N16" s="77"/>
       <c r="O16" s="37" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="P16" s="37"/>
     </row>
@@ -23148,7 +23450,7 @@
         <v>0.08945260347</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18">
@@ -23291,7 +23593,7 @@
         <v>0.1304926764</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="23">
@@ -24014,10 +24316,10 @@
         <v>0.05488621151</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="K48" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49">
@@ -24104,10 +24406,10 @@
         <v>0.06446991404</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="K51" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="52">
@@ -24138,7 +24440,7 @@
         <v>0.04492753623</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="53">
@@ -24441,7 +24743,7 @@
         <v>26.0</v>
       </c>
       <c r="I64" s="8">
-        <f t="shared" ref="I64:I67" si="5">(AVERAGE(G64:H64)/F64)</f>
+        <f t="shared" ref="I64:I68" si="5">(AVERAGE(G64:H64)/F64)</f>
         <v>0.02674897119</v>
       </c>
     </row>
@@ -24529,10 +24831,13 @@
         <v>0.1604046243</v>
       </c>
       <c r="J67" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="68">
+      <c r="A68" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="B68" s="4">
         <v>45212.0</v>
       </c>
@@ -24544,11 +24849,23 @@
         <v>4.0</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="G68" s="91"/>
+        <v>146</v>
+      </c>
+      <c r="F68" s="7">
+        <v>775.0</v>
+      </c>
+      <c r="G68" s="89">
+        <v>94.0</v>
+      </c>
+      <c r="I68" s="8">
+        <f t="shared" si="5"/>
+        <v>0.1212903226</v>
+      </c>
     </row>
     <row r="69">
+      <c r="A69" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="B69" s="4">
         <v>45213.0</v>
       </c>
@@ -24560,29 +24877,146 @@
         <v>4.0</v>
       </c>
       <c r="E69" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G69" s="91"/>
+      <c r="I69" s="8"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B70" s="4">
+        <v>45214.0</v>
+      </c>
+      <c r="C70" s="14">
+        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
+      <c r="D70" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G70" s="91"/>
+      <c r="I70" s="8"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B71" s="4">
+        <v>45215.0</v>
+      </c>
+      <c r="C71" s="14">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="D71" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E71" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="G69" s="91"/>
-    </row>
-    <row r="70">
-      <c r="G70" s="91"/>
-    </row>
-    <row r="71">
-      <c r="G71" s="91"/>
+      <c r="F71" s="7">
+        <v>566.0</v>
+      </c>
+      <c r="G71" s="89">
+        <v>95.0</v>
+      </c>
+      <c r="I71" s="8">
+        <f t="shared" ref="I71:I72" si="6">(AVERAGE(G71:H71)/F71)</f>
+        <v>0.167844523</v>
+      </c>
     </row>
     <row r="72">
-      <c r="G72" s="91"/>
+      <c r="A72" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="4">
+        <v>45216.0</v>
+      </c>
+      <c r="C72" s="14">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="D72" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F72" s="7">
+        <v>1125.0</v>
+      </c>
+      <c r="G72" s="89">
+        <v>67.0</v>
+      </c>
+      <c r="I72" s="8">
+        <f t="shared" si="6"/>
+        <v>0.05955555556</v>
+      </c>
     </row>
     <row r="73">
+      <c r="A73" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B73" s="4">
+        <v>45217.0</v>
+      </c>
+      <c r="C73" s="14">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="D73" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="G73" s="91"/>
     </row>
     <row r="74">
+      <c r="B74" s="4">
+        <v>45218.0</v>
+      </c>
+      <c r="C74" s="14">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="D74" s="95">
+        <v>4.0</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>148</v>
+      </c>
       <c r="G74" s="91"/>
     </row>
     <row r="75">
+      <c r="B75" s="4">
+        <v>45219.0</v>
+      </c>
+      <c r="C75" s="14">
+        <f t="shared" si="2"/>
+        <v>74</v>
+      </c>
+      <c r="D75" s="95">
+        <v>4.0</v>
+      </c>
       <c r="G75" s="91"/>
     </row>
     <row r="76">
+      <c r="B76" s="4">
+        <v>45220.0</v>
+      </c>
+      <c r="C76" s="14">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="D76" s="95">
+        <v>4.0</v>
+      </c>
       <c r="G76" s="91"/>
     </row>
     <row r="77">
@@ -24715,10 +25149,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="73" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H1" s="73" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I1" s="87" t="s">
         <v>7</v>
@@ -24772,16 +25206,16 @@
         <v>11</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="Q2" s="17" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3">
@@ -24792,7 +25226,7 @@
         <v>45147.0</v>
       </c>
       <c r="C3" s="14">
-        <f t="shared" ref="C3:C71" si="2">C2+1</f>
+        <f t="shared" ref="C3:C76" si="2">C2+1</f>
         <v>2</v>
       </c>
       <c r="D3" s="15">
@@ -24904,7 +25338,7 @@
         <v>0.09290322581</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M5" s="18" t="s">
         <v>16</v>
@@ -24950,7 +25384,7 @@
         <v>0.09449760766</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M6" s="25" t="s">
         <v>183</v>
@@ -24996,7 +25430,7 @@
         <v>0.06090373281</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="M7" s="25" t="s">
         <v>22</v>
@@ -25042,7 +25476,7 @@
         <v>0.0527325024</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="M8" s="26" t="s">
         <v>26</v>
@@ -25088,7 +25522,7 @@
         <v>0.07843137255</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M9" s="18" t="s">
         <v>28</v>
@@ -25134,7 +25568,7 @@
         <v>0.05448717949</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M10" s="25" t="s">
         <v>188</v>
@@ -25180,7 +25614,7 @@
         <v>0.0797752809</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="M11" s="25" t="s">
         <v>35</v>
@@ -25226,7 +25660,7 @@
         <v>0.1052631579</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M12" s="18" t="s">
         <v>37</v>
@@ -25272,7 +25706,7 @@
         <v>0.09417596035</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="M13" s="29" t="s">
         <v>40</v>
@@ -25318,7 +25752,7 @@
         <v>0.1331403763</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="M14" s="30" t="s">
         <v>43</v>
@@ -25413,7 +25847,7 @@
         <v>45041.0</v>
       </c>
       <c r="O16" s="37" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="P16" s="37"/>
     </row>
@@ -25896,7 +26330,7 @@
         <v>0.008875739645</v>
       </c>
       <c r="J33" s="23" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34">
@@ -26301,10 +26735,10 @@
         <v>0.135</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="K48" s="99" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49">
@@ -26391,10 +26825,10 @@
         <v>0.1600688468</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="K51" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="52">
@@ -26484,7 +26918,7 @@
         <v>0.2111553785</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="55">
@@ -26571,7 +27005,7 @@
         <v>0.2033096927</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="58">
@@ -26630,10 +27064,10 @@
         <v>0.3072916667</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="K59" s="7" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="60">
@@ -26664,7 +27098,7 @@
         <v>0.007702182285</v>
       </c>
       <c r="J60" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="61">
@@ -26757,7 +27191,7 @@
         <v>0.0</v>
       </c>
       <c r="I64" s="8">
-        <f t="shared" ref="I64:I67" si="4">(AVERAGE(G64:H64)/F64)</f>
+        <f t="shared" ref="I64:I68" si="4">(AVERAGE(G64:H64)/F64)</f>
         <v>0</v>
       </c>
     </row>
@@ -26845,10 +27279,13 @@
         <v>0.1166666667</v>
       </c>
       <c r="J67" s="7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="68">
+      <c r="A68" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B68" s="4">
         <v>45212.0</v>
       </c>
@@ -26860,10 +27297,23 @@
         <v>4.0</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
+      </c>
+      <c r="F68" s="7">
+        <v>375.0</v>
+      </c>
+      <c r="G68" s="7">
+        <v>49.0</v>
+      </c>
+      <c r="I68" s="8">
+        <f t="shared" si="4"/>
+        <v>0.1306666667</v>
       </c>
     </row>
     <row r="69">
+      <c r="A69" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B69" s="4">
         <v>45213.0</v>
       </c>
@@ -26875,10 +27325,14 @@
         <v>4.0</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>146</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="I69" s="8"/>
     </row>
     <row r="70">
+      <c r="A70" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="B70" s="4">
         <v>45214.0</v>
       </c>
@@ -26889,8 +27343,15 @@
       <c r="D70" s="98">
         <v>4.0</v>
       </c>
+      <c r="E70" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="I70" s="8"/>
     </row>
     <row r="71">
+      <c r="A71" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B71" s="4">
         <v>45215.0</v>
       </c>
@@ -26899,6 +27360,113 @@
         <v>70</v>
       </c>
       <c r="D71" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F71" s="7">
+        <v>336.0</v>
+      </c>
+      <c r="G71" s="7">
+        <v>75.0</v>
+      </c>
+      <c r="I71" s="8">
+        <f t="shared" ref="I71:I72" si="5">(AVERAGE(G71:H71)/F71)</f>
+        <v>0.2232142857</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="4">
+        <v>45216.0</v>
+      </c>
+      <c r="C72" s="14">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="D72" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F72" s="7">
+        <v>432.0</v>
+      </c>
+      <c r="G72" s="7">
+        <v>19.0</v>
+      </c>
+      <c r="I72" s="8">
+        <f t="shared" si="5"/>
+        <v>0.04398148148</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B73" s="4">
+        <v>45217.0</v>
+      </c>
+      <c r="C73" s="14">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="D73" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74" s="4">
+        <v>45218.0</v>
+      </c>
+      <c r="C74" s="14">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="D74" s="98">
+        <v>4.0</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" s="4">
+        <v>45219.0</v>
+      </c>
+      <c r="C75" s="14">
+        <f t="shared" si="2"/>
+        <v>74</v>
+      </c>
+      <c r="D75" s="98">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" s="4">
+        <v>45220.0</v>
+      </c>
+      <c r="C76" s="14">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="D76" s="98">
         <v>4.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating code for pokes
</commit_message>
<xml_diff>
--- a/juan/coop_seek_and_find_v2_updated.xlsx
+++ b/juan/coop_seek_and_find_v2_updated.xlsx
@@ -1498,7 +1498,7 @@
     <xdr:ext cx="4200525" cy="3143250"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image13.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1539,7 +1539,7 @@
     <xdr:ext cx="3752850" cy="2962275"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1572,7 +1572,7 @@
     <xdr:ext cx="3781425" cy="3048000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1609,7 +1609,7 @@
     <xdr:ext cx="3810000" cy="3000375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1637,7 +1637,7 @@
     <xdr:ext cx="4695825" cy="3000375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image15.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image14.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1665,7 +1665,7 @@
     <xdr:ext cx="5829300" cy="3000375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image11.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1693,7 +1693,7 @@
     <xdr:ext cx="4152900" cy="3571875"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1721,7 +1721,7 @@
     <xdr:ext cx="3714750" cy="3248025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1749,7 +1749,7 @@
     <xdr:ext cx="4152900" cy="3629025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1782,7 +1782,7 @@
     <xdr:ext cx="3781425" cy="3095625"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1810,7 +1810,7 @@
     <xdr:ext cx="4676775" cy="3476625"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1871,7 +1871,7 @@
     <xdr:ext cx="3781425" cy="2847975"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1899,7 +1899,7 @@
     <xdr:ext cx="3829050" cy="2924175"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image13.png" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image15.png" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5720,7 +5720,7 @@
         <v>6.0</v>
       </c>
       <c r="I72" s="8">
-        <f t="shared" ref="I72:I74" si="5">(AVERAGE(G72:H72)/F72)</f>
+        <f t="shared" ref="I72:I76" si="5">(AVERAGE(G72:H72)/F72)</f>
         <v>0.01058201058</v>
       </c>
     </row>
@@ -5797,6 +5797,16 @@
       <c r="E75" s="7" t="s">
         <v>224</v>
       </c>
+      <c r="F75" s="7">
+        <v>411.0</v>
+      </c>
+      <c r="G75" s="7">
+        <v>4.0</v>
+      </c>
+      <c r="I75" s="8">
+        <f t="shared" si="5"/>
+        <v>0.009732360097</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="7" t="s">
@@ -5814,6 +5824,16 @@
       </c>
       <c r="E76" s="7" t="s">
         <v>148</v>
+      </c>
+      <c r="F76" s="7">
+        <v>677.0</v>
+      </c>
+      <c r="G76" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="I76" s="8">
+        <f t="shared" si="5"/>
+        <v>0.004431314623</v>
       </c>
     </row>
     <row r="77">

</xml_diff>